<commit_message>
Add CAPEX annualization file
</commit_message>
<xml_diff>
--- a/GenX_sims/sim1.4_final/all_model_inputs.xlsx
+++ b/GenX_sims/sim1.4_final/all_model_inputs.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spenceregan/Repos/CU/Future_Power_Grid/Project2/GenX_sims/sim1.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spenceregan/GenX/SCPA/Sim5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26588AFC-D74C-9341-AAEB-33F8C37579D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6BFF58-850D-AC4E-B629-D4C0ED51B261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41140" yWindow="7480" windowWidth="26840" windowHeight="12080" xr2:uid="{CD31797F-9873-734C-9B3D-1C14D3F8E93B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CD31797F-9873-734C-9B3D-1C14D3F8E93B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Generator</t>
   </si>
@@ -87,16 +87,20 @@
   </si>
   <si>
     <t>Net Capital Cost</t>
+  </si>
+  <si>
+    <t>Geothermal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -142,7 +146,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -150,7 +154,8 @@
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -160,6 +165,15 @@
   <dxfs count="5">
     <dxf>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -178,16 +192,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -225,8 +230,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D2E6F903-8BA5-9F44-AAB5-BFD6368091E2}" name="Table1" displayName="Table1" ref="A1:I7" totalsRowShown="0">
-  <autoFilter ref="A1:I7" xr:uid="{D2E6F903-8BA5-9F44-AAB5-BFD6368091E2}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D2E6F903-8BA5-9F44-AAB5-BFD6368091E2}" name="Table1" displayName="Table1" ref="A1:I8" totalsRowShown="0">
+  <autoFilter ref="A1:I8" xr:uid="{D2E6F903-8BA5-9F44-AAB5-BFD6368091E2}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -243,10 +248,10 @@
     <tableColumn id="8" xr3:uid="{2D162BA9-9706-094F-8DFE-B08C758E03A2}" name="Direct Pay ITC" dataDxfId="3" dataCellStyle="Percent">
       <calculatedColumnFormula>0.3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{1326DBDA-37AD-A14D-A148-956782010AA3}" name="Net Capital Cost" dataDxfId="1" dataCellStyle="Currency">
+    <tableColumn id="9" xr3:uid="{1326DBDA-37AD-A14D-A148-956782010AA3}" name="Net Capital Cost" dataDxfId="2" dataCellStyle="Currency">
       <calculatedColumnFormula>(1-Table1[[#This Row],[Direct Pay ITC]])*Table1[[#This Row],[$/MW Gross Capital Cost]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{1459F485-5D90-124F-A243-31A0C4AB737C}" name="Annual Rate" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{1459F485-5D90-124F-A243-31A0C4AB737C}" name="Annual Rate" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{FA2B7E94-1754-4941-B690-CE990D197124}" name="Term"/>
     <tableColumn id="5" xr3:uid="{0D7A95F4-A61C-F34A-A7B6-93BF5AA18629}" name="$/MW/yr" dataDxfId="0">
       <calculatedColumnFormula>PMT(Table1[[#This Row],[Annual Rate]],Table1[[#This Row],[Term]],Table1[[#This Row],[Net Capital Cost]])</calculatedColumnFormula>
@@ -555,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C31249-83D9-1048-8F06-A66735A3BCD4}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -566,7 +571,7 @@
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
     <col min="2" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="38" customWidth="1"/>
   </cols>
   <sheetData>
@@ -776,10 +781,59 @@
         <v>11</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="8">
+        <v>38816715</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="D8" s="7">
+        <f>(1-Table1[[#This Row],[Direct Pay ITC]])*Table1[[#This Row],[$/MW Gross Capital Cost]]</f>
+        <v>27171700.5</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="F8">
+        <v>30</v>
+      </c>
+      <c r="G8" s="2">
+        <f>PMT(Table1[[#This Row],[Annual Rate]],Table1[[#This Row],[Term]],Table1[[#This Row],[Net Capital Cost]])</f>
+        <v>-1368420.751393327</v>
+      </c>
+    </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10">
         <f>B5*60/1000000</f>
         <v>8.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <f>B8/1000</f>
+        <v>38816.714999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <f>495631/2</f>
+        <v>247815.5</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G17" s="2">
+        <f>G8/(0.8*8760)</f>
+        <v>-195.26551817827155</v>
+      </c>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G20" s="2">
+        <f>G15-G17</f>
+        <v>248010.76551817826</v>
       </c>
     </row>
   </sheetData>

</xml_diff>